<commit_message>
extra arrows after each comment in the code were suddenly there so needed to be deleted. FInal rpesentation nearly finished
</commit_message>
<xml_diff>
--- a/Computing Practice - comp1004/Work/Sprint backlog/Sprint backlog table.xlsx
+++ b/Computing Practice - comp1004/Work/Sprint backlog/Sprint backlog table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Comp-1004---Computing-Practice\Computing Practice - comp1004\1 - Planning\Sprint backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Github\COMP1004 - HTML-CSS-and-JAVA\Computing Practice - comp1004\Work\Sprint backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECEDC39-A71F-4CAA-A92E-B45DC61FC14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4468C90A-A464-4285-8D65-BA7331E955B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{5BC79AD4-BCD0-4F44-BA86-801BFBD84420}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5BC79AD4-BCD0-4F44-BA86-801BFBD84420}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprints" sheetId="1" r:id="rId1"/>
@@ -534,20 +534,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA5CEF5-34FB-4995-AC0E-1736528F3859}">
   <dimension ref="A2:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.59765625" customWidth="1"/>
-    <col min="2" max="2" width="8.796875" customWidth="1"/>
-    <col min="3" max="3" width="52.1328125" customWidth="1"/>
-    <col min="4" max="4" width="39.796875" customWidth="1"/>
-    <col min="5" max="5" width="123.06640625" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="52.109375" customWidth="1"/>
+    <col min="4" max="4" width="39.77734375" customWidth="1"/>
+    <col min="5" max="5" width="123.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -564,7 +564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -581,7 +581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="33.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -598,7 +598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="77.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="77.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -615,7 +615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="61.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -632,7 +632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -649,7 +649,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="72.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="72.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -666,7 +666,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="106.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -683,7 +683,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="49.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>

</xml_diff>